<commit_message>
Code pushed from office system
</commit_message>
<xml_diff>
--- a/Configuration/Experts-Staging-TestData-ExcelSheet2.xlsx
+++ b/Configuration/Experts-Staging-TestData-ExcelSheet2.xlsx
@@ -45,13 +45,13 @@
     <t>Email</t>
   </si>
   <si>
-    <t>mayur.charvande+1@fxbytes.com</t>
-  </si>
-  <si>
-    <t>mayur.charvande+2@fxbytes.com</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mobile Number </t>
+  </si>
+  <si>
+    <t>mayur.charvande+3@fxbytes.com</t>
+  </si>
+  <si>
+    <t>mayur.charvande+4@fxbytes.com</t>
   </si>
 </sst>
 </file>
@@ -413,7 +413,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,7 +421,7 @@
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
     <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="31.85546875" customWidth="1"/>
+    <col min="4" max="4" width="34.28515625" customWidth="1"/>
     <col min="5" max="5" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -439,7 +439,7 @@
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -453,7 +453,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E2">
         <v>7620248349</v>

</xml_diff>

<commit_message>
uploaded from office system
</commit_message>
<xml_diff>
--- a/Configuration/Experts-Staging-TestData-ExcelSheet2.xlsx
+++ b/Configuration/Experts-Staging-TestData-ExcelSheet2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>FirstName</t>
   </si>
@@ -48,10 +48,22 @@
     <t xml:space="preserve">Mobile Number </t>
   </si>
   <si>
-    <t>mayur.charvande+3@fxbytes.com</t>
-  </si>
-  <si>
-    <t>mayur.charvande+4@fxbytes.com</t>
+    <t>Country code</t>
+  </si>
+  <si>
+    <t>mayur.charvande+4@fxbytes1.com</t>
+  </si>
+  <si>
+    <t>mayur.charvande+3@fxbytes2.com</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Devas Naka, Indore</t>
+  </si>
+  <si>
+    <t>Pune</t>
   </si>
 </sst>
 </file>
@@ -104,10 +116,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -410,22 +429,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="34.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="13" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="34.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="27.85546875" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -441,39 +463,57 @@
       <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>7620248349</v>
       </c>
+      <c r="F2" s="2">
+        <v>91</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3">
+      <c r="D3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2">
         <v>7045827283</v>
+      </c>
+      <c r="F3" s="2">
+        <v>92</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -484,6 +524,7 @@
     <hyperlink ref="D3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>